<commit_message>
roberta's robustness test results
</commit_message>
<xml_diff>
--- a/experiments/evaluation/llm-based/roberta-base_15/original_remove/rem1/correct_predictions.xlsx
+++ b/experiments/evaluation/llm-based/roberta-base_15/original_remove/rem1/correct_predictions.xlsx
@@ -467,7 +467,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -497,7 +497,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -527,7 +527,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>

</xml_diff>